<commit_message>
Fix bug Role, Add Status > Book, BookCate DBInitializer, fix Book, BookCate seed data
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="41">
   <si>
     <t>Id</t>
   </si>
@@ -128,6 +128,15 @@
   </si>
   <si>
     <t xml:space="preserve">AdContract </t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Add col "Loại" but can't load the FKNavigation data</t>
   </si>
 </sst>
 </file>
@@ -481,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -900,7 +909,7 @@
         <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
@@ -923,7 +932,7 @@
         <v>32</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
@@ -946,7 +955,7 @@
         <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
@@ -975,6 +984,24 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add edit book status
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -136,7 +136,7 @@
     <t>User</t>
   </si>
   <si>
-    <t>Add col "Loại" but can't load the FKNavigation data</t>
+    <t>Add col "Loại" but can't load the FKNavigation data, don't know how</t>
   </si>
 </sst>
 </file>
@@ -491,14 +491,14 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="51.375" customWidth="1"/>
+    <col min="4" max="4" width="56.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.75" customWidth="1"/>
     <col min="7" max="7" width="12.25" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Fix Delivery, Add function for Merchant to update Delivery,
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="45">
   <si>
     <t>Id</t>
   </si>
@@ -137,6 +137,19 @@
   </si>
   <si>
     <t>Add col "Loại" but can't load the FKNavigation data, don't know how</t>
+  </si>
+  <si>
+    <t>M-Update status and update totalprice</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Add UpdateStatus function (Select oneway_clientside)</t>
+  </si>
+  <si>
+    <t>After Customer order successfully &gt; create Delivery: status: Unconfirm, Ship = 0, TotalPrice=0.
+calculate OrderPrice plz.</t>
   </si>
 </sst>
 </file>
@@ -181,9 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,20 +504,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="10.875" customWidth="1"/>
-    <col min="4" max="4" width="56.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="68.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.75" customWidth="1"/>
-    <col min="7" max="7" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -725,10 +741,10 @@
         <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F10" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
@@ -863,10 +879,10 @@
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -1001,6 +1017,75 @@
         <v>9</v>
       </c>
       <c r="G22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
.load UserType .Import general
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="47">
   <si>
     <t>Id</t>
   </si>
@@ -150,6 +150,12 @@
   <si>
     <t>After Customer order successfully &gt; create Delivery: status: Unconfirm, Ship = 0, TotalPrice=0.
 calculate OrderPrice plz.</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Load Img: /&lt;merchantName&gt;/Books/&lt;BookId.&lt;pnj/jpeg&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -606,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
@@ -1086,6 +1092,26 @@
         <v>38</v>
       </c>
       <c r="G25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add UploadImg Book (not done yet) Fix money bug
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="52">
   <si>
     <t>Id</t>
   </si>
@@ -156,6 +156,21 @@
   </si>
   <si>
     <t>Load Img: /&lt;merchantName&gt;/Books/&lt;BookId.&lt;pnj/jpeg&gt;&gt;</t>
+  </si>
+  <si>
+    <t>AdContent vs AdContract still not done</t>
+  </si>
+  <si>
+    <t>Advertisement</t>
+  </si>
+  <si>
+    <t>Seed data for AdContent vs AdContract</t>
+  </si>
+  <si>
+    <t>Upload file Img: validate file extension,…..</t>
+  </si>
+  <si>
+    <t>Show Gender</t>
   </si>
 </sst>
 </file>
@@ -510,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1020,7 +1035,7 @@
         <v>14</v>
       </c>
       <c r="F22" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G22" t="s">
         <v>10</v>
@@ -1096,6 +1111,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
@@ -1109,10 +1127,177 @@
         <v>14</v>
       </c>
       <c r="F26" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G26" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix sort by Status (M + C) Fix sort by Scale (M) Fix bugs
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="54">
   <si>
     <t>Id</t>
   </si>
@@ -171,6 +171,12 @@
   </si>
   <si>
     <t>Show Gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can't update to table User </t>
+  </si>
+  <si>
+    <t>change MerchantCompanyName?</t>
   </si>
 </sst>
 </file>
@@ -527,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -581,7 +587,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -650,7 +656,7 @@
         <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -1219,7 +1225,7 @@
         <v>14</v>
       </c>
       <c r="F30" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G30" t="s">
         <v>10</v>
@@ -1229,10 +1235,46 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix sort by Status (WM)
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -679,7 +679,7 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
@@ -748,7 +748,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Fix sort by Position, Status (WM) Fix bugs
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -201,12 +201,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -221,12 +233,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,14 +547,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.75" customWidth="1"/>
@@ -570,118 +585,118 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="F2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="F4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="F6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -731,49 +746,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="F9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="F10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -823,26 +838,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="F13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -869,49 +884,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="F15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="F16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -935,72 +950,72 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="F18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F19" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="F19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1024,26 +1039,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" t="s">
+      <c r="E22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1093,49 +1108,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="B25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E25" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="E25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G26" t="s">
+      <c r="E26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1208,26 +1223,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E30" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="E30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix sort by Status (AdPosition)
</commit_message>
<xml_diff>
--- a/Project's bugs.xlsx
+++ b/Project's bugs.xlsx
@@ -548,7 +548,7 @@
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -815,26 +815,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
@@ -944,7 +944,7 @@
         <v>14</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>

</xml_diff>